<commit_message>
Add Book code is added enter_book_detail method is created and added new csv file called book_details.
</commit_message>
<xml_diff>
--- a/MainAssignment/DataFile/Login_details.xlsx
+++ b/MainAssignment/DataFile/Login_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -77,6 +77,24 @@
   </si>
   <si>
     <t>ASDFGHJK</t>
+  </si>
+  <si>
+    <t>khanbb</t>
+  </si>
+  <si>
+    <t>sad123</t>
+  </si>
+  <si>
+    <t>band123</t>
+  </si>
+  <si>
+    <t>dand321</t>
+  </si>
+  <si>
+    <t>khankhankhan</t>
+  </si>
+  <si>
+    <t>123456789</t>
   </si>
 </sst>
 </file>
@@ -529,6 +547,39 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>